<commit_message>
Datos base, y estimación de datos totales
</commit_message>
<xml_diff>
--- a/SizeTableSpace.xlsx
+++ b/SizeTableSpace.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\University\2023-2\CABDR\GestorEmpleados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anmon\OneDrive\Documentos\Repositories\BDEmpleados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD508023-1286-4F02-8CB9-2B027D33564E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DB27E013-AF8E-423F-AC03-95205CBDD9B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -113,8 +112,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +123,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,14 +222,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,10 +239,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,385 +562,394 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0AA143-94E0-4059-9BA5-64A356483FC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D1" s="3" t="s">
+    <row r="1" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F3" s="9">
-        <v>64</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="E3" s="4">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4">
+        <v>64</v>
+      </c>
+      <c r="G3" s="4">
         <f>E3*F3</f>
-        <v>6400000</v>
-      </c>
-      <c r="H3" s="9">
+        <v>448</v>
+      </c>
+      <c r="H3" s="4">
         <f>G3 / 1024</f>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F4" s="9">
-        <v>10240</v>
-      </c>
-      <c r="G4" s="9">
-        <f t="shared" ref="G4:G19" si="0">E4*F4</f>
-        <v>1024000000</v>
-      </c>
-      <c r="H4" s="9">
-        <f t="shared" ref="H4:H19" si="1">G4 / 1024</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <f>E6</f>
+        <v>3670.7999999999993</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1024</v>
+      </c>
+      <c r="G4" s="4">
+        <f>E4*F4</f>
+        <v>3758899.1999999993</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" ref="H4:H19" si="0">G4 / 1024</f>
+        <v>3670.7999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F5" s="9">
-        <v>10240</v>
-      </c>
-      <c r="G5" s="9">
-        <f t="shared" si="0"/>
-        <v>1024000000</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E5" s="4">
+        <f>3*E4</f>
+        <v>11012.399999999998</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1024</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G4:G19" si="1">E5*F5</f>
+        <v>11276697.599999998</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>11012.399999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F6" s="9">
-        <v>10240</v>
-      </c>
-      <c r="G6" s="9">
-        <f t="shared" si="0"/>
-        <v>1024000000</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <f>0.95*E14</f>
+        <v>3670.7999999999993</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1024</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>3758899.1999999993</v>
+      </c>
+      <c r="H6" s="4">
+        <f>G6 / 1024</f>
+        <v>3670.7999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F7" s="9">
-        <v>64</v>
-      </c>
-      <c r="G7" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="F7" s="4">
+        <v>64</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>3840</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F8" s="9">
-        <v>64</v>
-      </c>
-      <c r="G8" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H8" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E8" s="4">
+        <f>E7*E12*0.65</f>
+        <v>2340</v>
+      </c>
+      <c r="F8" s="4">
+        <v>64</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>149760</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="0"/>
+        <v>146.25</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="9">
-        <v>100000</v>
+      <c r="E9" s="4">
+        <v>2</v>
       </c>
       <c r="F9" s="9">
         <v>64</v>
       </c>
-      <c r="G9" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G9" s="4">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F10" s="9">
-        <v>64</v>
-      </c>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>64</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F11" s="9">
+      <c r="E11" s="4">
+        <f>0.2*E4</f>
+        <v>734.15999999999985</v>
+      </c>
+      <c r="F11" s="4">
         <v>5120</v>
       </c>
-      <c r="G11" s="9">
-        <f t="shared" si="0"/>
-        <v>512000000</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="1"/>
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>3758899.1999999993</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>3670.7999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F12" s="9">
-        <v>64</v>
-      </c>
-      <c r="G12" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="4">
+        <v>60</v>
+      </c>
+      <c r="F12" s="4">
+        <v>64</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
+        <v>3840</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F13" s="9">
-        <v>64</v>
-      </c>
-      <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E13" s="4">
+        <f>E12*E16*0.7</f>
+        <v>840</v>
+      </c>
+      <c r="F13" s="4">
+        <v>64</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
+        <v>53760</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F14" s="9">
-        <v>10240</v>
-      </c>
-      <c r="G14" s="9">
-        <f t="shared" si="0"/>
-        <v>1024000000</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="4">
+        <f>(4*E13)*1.15</f>
+        <v>3863.9999999999995</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1024</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="1"/>
+        <v>3956735.9999999995</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="0"/>
+        <v>3863.9999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F15" s="9">
-        <v>10240</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="0"/>
-        <v>1024000000</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="shared" si="1"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <f>E4</f>
+        <v>3670.7999999999993</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1024</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>3758899.1999999993</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>3670.7999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F16" s="9">
-        <v>64</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="10">
+        <v>20</v>
+      </c>
+      <c r="F16" s="4">
+        <v>64</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>1280</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F17" s="9">
-        <v>64</v>
-      </c>
-      <c r="G17" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H17" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="4">
+        <v>20</v>
+      </c>
+      <c r="F17" s="4">
+        <v>64</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="1"/>
+        <v>1280</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F18" s="9">
-        <v>64</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H18" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4">
+        <v>64</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="9">
-        <v>100000</v>
-      </c>
-      <c r="F19" s="9">
-        <v>64</v>
-      </c>
-      <c r="G19" s="9">
-        <f t="shared" si="0"/>
-        <v>6400000</v>
-      </c>
-      <c r="H19" s="9">
-        <f t="shared" si="1"/>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
+        <v>6</v>
+      </c>
+      <c r="F19" s="4">
+        <v>64</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="8">
+      <c r="H20" s="11">
         <f>SUM(H3:H19)</f>
-        <v>5568750</v>
+        <v>29769.537499999995</v>
       </c>
     </row>
   </sheetData>
@@ -936,5 +958,6 @@
     <mergeCell ref="D1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>